<commit_message>
update sign in functionality
</commit_message>
<xml_diff>
--- a/src/test/resources/exceldata/signInTestData.xlsx
+++ b/src/test/resources/exceldata/signInTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anil.basudkar\eclipse-workspace\DSAlgo-FourPetal\src\test\resources\exceldata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D0D38C9-1799-413F-8429-6BCF2F66ACC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B02123B-4D8B-411D-BCB0-78C6162E53AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1FD4E7A1-E67F-492A-9164-9DAFBB647B71}"/>
+    <workbookView xWindow="1480" yWindow="1480" windowWidth="14400" windowHeight="7360" xr2:uid="{1FD4E7A1-E67F-492A-9164-9DAFBB647B71}"/>
   </bookViews>
   <sheets>
     <sheet name="signIn" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
     <t>kanchanbasudkar</t>
   </si>
   <si>
-    <t>kanbas$</t>
+    <t>kanbas123$</t>
   </si>
 </sst>
 </file>
@@ -402,7 +402,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" activeCellId="1" sqref="A3 C8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
updated signIn negative test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/exceldata/signInTestData.xlsx
+++ b/src/test/resources/exceldata/signInTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anil.basudkar\eclipse-workspace\DSAlgo-FourPetal\src\test\resources\exceldata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B02123B-4D8B-411D-BCB0-78C6162E53AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E434CD0-C79F-4BFE-84D5-AC04291209D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1480" yWindow="1480" windowWidth="14400" windowHeight="7360" xr2:uid="{1FD4E7A1-E67F-492A-9164-9DAFBB647B71}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1FD4E7A1-E67F-492A-9164-9DAFBB647B71}"/>
   </bookViews>
   <sheets>
     <sheet name="signIn" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>userName</t>
   </si>
@@ -48,6 +48,27 @@
   </si>
   <si>
     <t>kanbas123$</t>
+  </si>
+  <si>
+    <t>kanasfdasabas123$</t>
+  </si>
+  <si>
+    <t>expectedmsg</t>
+  </si>
+  <si>
+    <t>You are logged in</t>
+  </si>
+  <si>
+    <t>Invalid Username and Password</t>
+  </si>
+  <si>
+    <t>kannnnn</t>
+  </si>
+  <si>
+    <t>Please fill out this field</t>
+  </si>
+  <si>
+    <t>hhojj</t>
   </si>
 </sst>
 </file>
@@ -399,28 +420,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07503148-E207-4B49-925E-8E14C48C1AF7}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.81640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>